<commit_message>
modified:   SECTOR_ETF/ETF_Result.xlsx 	new file:   SECTOR_ETF/KOSDAQ 100.xlsx 	new file:   SECTOR_ETF/excelBTsample.xlsx 	modified:   SECTOR_ETF/sectorETF_Ret&Vol.py 	modified:   "SECTOR_ETF/sectorETF_simple\354\241\260\355\225\251.py" 	modified:   "SECTOR_ETF/sectorETF_\353\263\200\353\217\231\354\204\261\353\217\214\355\214\214_Backtest_Fin.py" 	modified:   "SECTOR_ETF/\353\263\200\353\217\231\354\204\261\353\217\214\355\214\214Result.xlsx"
</commit_message>
<xml_diff>
--- a/SECTOR_ETF/변동성돌파Result.xlsx
+++ b/SECTOR_ETF/변동성돌파Result.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GSR\Desktop\Python_project\git_folder\SECTOR_ETF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01A926C-EA52-4597-BBA2-801AA2ED7C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2CF4F7-8412-4396-AAA7-0A1A040B2231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4245" yWindow="5385" windowWidth="28800" windowHeight="15420" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KODEX 200.xlsx" sheetId="1" r:id="rId1"/>
@@ -26,13 +26,14 @@
     <sheet name="TIGER 리츠부동산인프라.xlsx" sheetId="11" r:id="rId11"/>
     <sheet name="TIGER 헬스케어.xlsx" sheetId="12" r:id="rId12"/>
     <sheet name="TIGER 화장품.xlsx" sheetId="13" r:id="rId13"/>
+    <sheet name="KOSDAQ 100.xlsx" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1586" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1708" uniqueCount="17">
   <si>
     <t>Model</t>
   </si>
@@ -92,7 +93,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,8 +147,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,13 +166,34 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -221,7 +248,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -261,6 +288,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="176" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="백분율" xfId="1" builtinId="5"/>
@@ -7816,7 +7850,7 @@
   <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -9615,6 +9649,1818 @@
       </c>
       <c r="J56">
         <v>9.5643835616438349</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:J56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="11.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.25" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>0.4</v>
+      </c>
+      <c r="D2" s="5">
+        <v>15954.68423787443</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0.53586325709279992</v>
+      </c>
+      <c r="F2" s="5">
+        <v>-0.19814915556117441</v>
+      </c>
+      <c r="G2">
+        <v>2.2504733215903392</v>
+      </c>
+      <c r="H2">
+        <v>2.370462856354937</v>
+      </c>
+      <c r="I2">
+        <v>3312</v>
+      </c>
+      <c r="J2">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>0.3</v>
+      </c>
+      <c r="D3" s="5">
+        <v>21679.718862023241</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0.55688665031000695</v>
+      </c>
+      <c r="F3" s="5">
+        <v>-0.19454014182533</v>
+      </c>
+      <c r="G3">
+        <v>2.5742713761759899</v>
+      </c>
+      <c r="H3">
+        <v>2.3395796990517659</v>
+      </c>
+      <c r="I3">
+        <v>2745</v>
+      </c>
+      <c r="J3">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="18">
+        <v>0.4</v>
+      </c>
+      <c r="D4" s="19">
+        <v>11041.136798165269</v>
+      </c>
+      <c r="E4" s="19">
+        <v>0.51099787122328011</v>
+      </c>
+      <c r="F4" s="19">
+        <v>-0.1575137701357005</v>
+      </c>
+      <c r="G4" s="18">
+        <v>2.7442934543884858</v>
+      </c>
+      <c r="H4" s="18">
+        <v>2.3175929839447891</v>
+      </c>
+      <c r="I4" s="18">
+        <v>2244</v>
+      </c>
+      <c r="J4" s="18">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="5">
+        <v>9485.7980101125831</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.50085982172016141</v>
+      </c>
+      <c r="F5" s="5">
+        <v>-0.1956913194949092</v>
+      </c>
+      <c r="G5">
+        <v>2.2357266065626389</v>
+      </c>
+      <c r="H5">
+        <v>2.189935943378909</v>
+      </c>
+      <c r="I5">
+        <v>3015</v>
+      </c>
+      <c r="J5">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="D6" s="5">
+        <v>3939.3213960962712</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.44350396328219949</v>
+      </c>
+      <c r="F6" s="5">
+        <v>-0.1667773752698625</v>
+      </c>
+      <c r="G6">
+        <v>2.2683772540462228</v>
+      </c>
+      <c r="H6">
+        <v>2.1588437390045452</v>
+      </c>
+      <c r="I6">
+        <v>2511</v>
+      </c>
+      <c r="J6">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>0.6</v>
+      </c>
+      <c r="D7" s="5">
+        <v>5985.2494963521631</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.47052587487519387</v>
+      </c>
+      <c r="F7" s="5">
+        <v>-0.2041797162448824</v>
+      </c>
+      <c r="G7">
+        <v>2.2456720868246198</v>
+      </c>
+      <c r="H7">
+        <v>2.1495328165430858</v>
+      </c>
+      <c r="I7">
+        <v>2747</v>
+      </c>
+      <c r="J7">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="5">
+        <v>4356.6843270873169</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0.44996373320581567</v>
+      </c>
+      <c r="F8" s="5">
+        <v>-0.15032370725741559</v>
+      </c>
+      <c r="G8">
+        <v>2.7906203918625918</v>
+      </c>
+      <c r="H8">
+        <v>2.0988920569396572</v>
+      </c>
+      <c r="I8">
+        <v>1805</v>
+      </c>
+      <c r="J8">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>0.3</v>
+      </c>
+      <c r="D9" s="5">
+        <v>8998.3533156374342</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0.49735330154838331</v>
+      </c>
+      <c r="F9" s="5">
+        <v>-0.28441535899384263</v>
+      </c>
+      <c r="G9">
+        <v>1.944798093758439</v>
+      </c>
+      <c r="H9">
+        <v>2.0964154325464048</v>
+      </c>
+      <c r="I9">
+        <v>3686</v>
+      </c>
+      <c r="J9">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>0.2</v>
+      </c>
+      <c r="D10" s="5">
+        <v>12655.192690367559</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0.52016653732513984</v>
+      </c>
+      <c r="F10" s="5">
+        <v>-0.30671613556265709</v>
+      </c>
+      <c r="G10">
+        <v>2.0741298757992248</v>
+      </c>
+      <c r="H10">
+        <v>2.049826007243317</v>
+      </c>
+      <c r="I10">
+        <v>3419</v>
+      </c>
+      <c r="J10">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>0.8</v>
+      </c>
+      <c r="D11" s="5">
+        <v>2166.6778640068078</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0.40574430703285208</v>
+      </c>
+      <c r="F11" s="5">
+        <v>-0.17259718228069171</v>
+      </c>
+      <c r="G11">
+        <v>2.1886846845679391</v>
+      </c>
+      <c r="H11">
+        <v>2.0130679666284421</v>
+      </c>
+      <c r="I11">
+        <v>2342</v>
+      </c>
+      <c r="J11">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>0.6</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1237.999487806457</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0.3712878897335552</v>
+      </c>
+      <c r="F12" s="5">
+        <v>-0.1442984264306571</v>
+      </c>
+      <c r="G12">
+        <v>2.6786379231593371</v>
+      </c>
+      <c r="H12">
+        <v>2.0078840311916299</v>
+      </c>
+      <c r="I12">
+        <v>1504</v>
+      </c>
+      <c r="J12">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>0.9</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1300.026662142244</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.37426359089929417</v>
+      </c>
+      <c r="F13" s="5">
+        <v>-0.1881248774704497</v>
+      </c>
+      <c r="G13">
+        <v>2.1114920543579561</v>
+      </c>
+      <c r="H13">
+        <v>1.8477146623721099</v>
+      </c>
+      <c r="I13">
+        <v>2160</v>
+      </c>
+      <c r="J13">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>0.2</v>
+      </c>
+      <c r="D14" s="5">
+        <v>2322.8294280285281</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0.41008857807061538</v>
+      </c>
+      <c r="F14" s="5">
+        <v>-0.30982532439022098</v>
+      </c>
+      <c r="G14">
+        <v>1.4985270107993129</v>
+      </c>
+      <c r="H14">
+        <v>1.6754200818700751</v>
+      </c>
+      <c r="I14">
+        <v>4161</v>
+      </c>
+      <c r="J14">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>0.1</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1729.0768613926541</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0.3917524034601696</v>
+      </c>
+      <c r="F15" s="5">
+        <v>-0.40100004204717321</v>
+      </c>
+      <c r="G15">
+        <v>1.4023593621835919</v>
+      </c>
+      <c r="H15">
+        <v>1.5759153151739751</v>
+      </c>
+      <c r="I15">
+        <v>4249</v>
+      </c>
+      <c r="J15">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="D16" s="5">
+        <v>345.05533578400548</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0.29576983639062032</v>
+      </c>
+      <c r="F16" s="5">
+        <v>-0.14522358312873801</v>
+      </c>
+      <c r="G16">
+        <v>2.4481976163491921</v>
+      </c>
+      <c r="H16">
+        <v>1.546436611232072</v>
+      </c>
+      <c r="I16">
+        <v>1198</v>
+      </c>
+      <c r="J16">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <v>0.6</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1072.3470296805569</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0.36258165299432887</v>
+      </c>
+      <c r="F17" s="5">
+        <v>-0.34104571993081573</v>
+      </c>
+      <c r="G17">
+        <v>1.4517314459959469</v>
+      </c>
+      <c r="H17">
+        <v>1.432368563712169</v>
+      </c>
+      <c r="I17">
+        <v>3421</v>
+      </c>
+      <c r="J17">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="5">
+        <v>1064.713121900952</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0.36215009093123213</v>
+      </c>
+      <c r="F18" s="5">
+        <v>-0.4177049888485983</v>
+      </c>
+      <c r="G18">
+        <v>1.4020053267706241</v>
+      </c>
+      <c r="H18">
+        <v>1.4302833417525851</v>
+      </c>
+      <c r="I18">
+        <v>3633</v>
+      </c>
+      <c r="J18">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19">
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="D19" s="5">
+        <v>909.22900449370809</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0.3526489525305565</v>
+      </c>
+      <c r="F19" s="5">
+        <v>-0.36766569804079008</v>
+      </c>
+      <c r="G19">
+        <v>1.4666752392541971</v>
+      </c>
+      <c r="H19">
+        <v>1.4175424592087711</v>
+      </c>
+      <c r="I19">
+        <v>3235</v>
+      </c>
+      <c r="J19">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20">
+        <v>0.8</v>
+      </c>
+      <c r="D20" s="5">
+        <v>784.09123447961872</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0.34379739849133761</v>
+      </c>
+      <c r="F20" s="5">
+        <v>-0.38804774992835223</v>
+      </c>
+      <c r="G20">
+        <v>1.4736067914107189</v>
+      </c>
+      <c r="H20">
+        <v>1.3697354593970741</v>
+      </c>
+      <c r="I20">
+        <v>3061</v>
+      </c>
+      <c r="J20">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21">
+        <v>0.9</v>
+      </c>
+      <c r="D21" s="5">
+        <v>790.10263763707439</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0.34425253804542222</v>
+      </c>
+      <c r="F21" s="5">
+        <v>-0.34741783707885288</v>
+      </c>
+      <c r="G21">
+        <v>1.5151190125455369</v>
+      </c>
+      <c r="H21">
+        <v>1.349832671965385</v>
+      </c>
+      <c r="I21">
+        <v>2882</v>
+      </c>
+      <c r="J21">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22">
+        <v>0.1</v>
+      </c>
+      <c r="D22" s="5">
+        <v>545.51736126914125</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0.32235421832960842</v>
+      </c>
+      <c r="F22" s="5">
+        <v>-0.43798501664139777</v>
+      </c>
+      <c r="G22">
+        <v>1.117129105341871</v>
+      </c>
+      <c r="H22">
+        <v>1.345737811334869</v>
+      </c>
+      <c r="I22">
+        <v>4674</v>
+      </c>
+      <c r="J22">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <v>0.4</v>
+      </c>
+      <c r="D23" s="5">
+        <v>701.57346771092364</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0.33718810640292318</v>
+      </c>
+      <c r="F23" s="5">
+        <v>-0.47890551609671073</v>
+      </c>
+      <c r="G23">
+        <v>1.2604269639702581</v>
+      </c>
+      <c r="H23">
+        <v>1.32671637980788</v>
+      </c>
+      <c r="I23">
+        <v>3887</v>
+      </c>
+      <c r="J23">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24">
+        <v>0.3</v>
+      </c>
+      <c r="D24" s="5">
+        <v>477.60017499672</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0.31458139000934859</v>
+      </c>
+      <c r="F24" s="5">
+        <v>-0.50743160594572845</v>
+      </c>
+      <c r="G24">
+        <v>1.139316830160511</v>
+      </c>
+      <c r="H24">
+        <v>1.2499574085973599</v>
+      </c>
+      <c r="I24">
+        <v>4153</v>
+      </c>
+      <c r="J24">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25">
+        <v>0.2</v>
+      </c>
+      <c r="D25" s="5">
+        <v>305.86004653339722</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0.28886075957754481</v>
+      </c>
+      <c r="F25" s="5">
+        <v>-0.53220889279709094</v>
+      </c>
+      <c r="G25">
+        <v>1.0108511005608909</v>
+      </c>
+      <c r="H25">
+        <v>1.161866894421931</v>
+      </c>
+      <c r="I25">
+        <v>4468</v>
+      </c>
+      <c r="J25">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26">
+        <v>0.8</v>
+      </c>
+      <c r="D26" s="5">
+        <v>114.83047547160881</v>
+      </c>
+      <c r="E26" s="5">
+        <v>0.2340740295074564</v>
+      </c>
+      <c r="F26" s="5">
+        <v>-0.1184366006584099</v>
+      </c>
+      <c r="G26">
+        <v>2.147182402585575</v>
+      </c>
+      <c r="H26">
+        <v>1.13767536548253</v>
+      </c>
+      <c r="I26">
+        <v>958</v>
+      </c>
+      <c r="J26">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27">
+        <v>0.1</v>
+      </c>
+      <c r="D27" s="5">
+        <v>162.84477984134199</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0.25333798946253411</v>
+      </c>
+      <c r="F27" s="5">
+        <v>-0.51245666014818458</v>
+      </c>
+      <c r="G27">
+        <v>0.86203460886454863</v>
+      </c>
+      <c r="H27">
+        <v>1.05829218036475</v>
+      </c>
+      <c r="I27">
+        <v>4858</v>
+      </c>
+      <c r="J27">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28">
+        <v>0.5</v>
+      </c>
+      <c r="D28" s="5">
+        <v>17.040526606668472</v>
+      </c>
+      <c r="E28" s="5">
+        <v>0.1339735572625789</v>
+      </c>
+      <c r="F28" s="5">
+        <v>-0.1151853683852745</v>
+      </c>
+      <c r="G28">
+        <v>1.2900393937446799</v>
+      </c>
+      <c r="H28">
+        <v>1.0094170691482649</v>
+      </c>
+      <c r="I28">
+        <v>1805</v>
+      </c>
+      <c r="J28">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29">
+        <v>0.4</v>
+      </c>
+      <c r="D29" s="5">
+        <v>17.262151672821599</v>
+      </c>
+      <c r="E29" s="5">
+        <v>0.1346234500793424</v>
+      </c>
+      <c r="F29" s="5">
+        <v>-0.15214316824609561</v>
+      </c>
+      <c r="G29">
+        <v>1.1109900924846581</v>
+      </c>
+      <c r="H29">
+        <v>0.95617304286695504</v>
+      </c>
+      <c r="I29">
+        <v>2244</v>
+      </c>
+      <c r="J29">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30">
+        <v>0.9</v>
+      </c>
+      <c r="D30" s="5">
+        <v>55.732618953478067</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0.19514619666032831</v>
+      </c>
+      <c r="F30" s="5">
+        <v>-0.11344332488968541</v>
+      </c>
+      <c r="G30">
+        <v>1.9989634429285119</v>
+      </c>
+      <c r="H30">
+        <v>0.90094246165270253</v>
+      </c>
+      <c r="I30">
+        <v>754</v>
+      </c>
+      <c r="J30">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31">
+        <v>0.6</v>
+      </c>
+      <c r="D31" s="5">
+        <v>8.6129394951774199</v>
+      </c>
+      <c r="E31" s="5">
+        <v>0.10018021693756959</v>
+      </c>
+      <c r="F31" s="5">
+        <v>-0.13196031527794541</v>
+      </c>
+      <c r="G31">
+        <v>1.073126958403152</v>
+      </c>
+      <c r="H31">
+        <v>0.7660954538455188</v>
+      </c>
+      <c r="I31">
+        <v>1504</v>
+      </c>
+      <c r="J31">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32">
+        <v>0.3</v>
+      </c>
+      <c r="D32" s="5">
+        <v>10.91582216627067</v>
+      </c>
+      <c r="E32" s="5">
+        <v>0.1117997076498056</v>
+      </c>
+      <c r="F32" s="5">
+        <v>-0.27886985845417139</v>
+      </c>
+      <c r="G32">
+        <v>0.76970288094687644</v>
+      </c>
+      <c r="H32">
+        <v>0.70918022751886212</v>
+      </c>
+      <c r="I32">
+        <v>2745</v>
+      </c>
+      <c r="J32">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33">
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="D33" s="5">
+        <v>7.4956608879548092</v>
+      </c>
+      <c r="E33" s="5">
+        <v>9.3423342918440566E-2</v>
+      </c>
+      <c r="F33" s="5">
+        <v>-8.4824950818125341E-2</v>
+      </c>
+      <c r="G33">
+        <v>1.1360677148671321</v>
+      </c>
+      <c r="H33">
+        <v>0.70515283005390283</v>
+      </c>
+      <c r="I33">
+        <v>1198</v>
+      </c>
+      <c r="J33">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34">
+        <v>0.8</v>
+      </c>
+      <c r="D34" s="5">
+        <v>5.847323092547219</v>
+      </c>
+      <c r="E34" s="5">
+        <v>8.1449480719449907E-2</v>
+      </c>
+      <c r="F34" s="5">
+        <v>-8.7515477894879914E-2</v>
+      </c>
+      <c r="G34">
+        <v>1.100669391314294</v>
+      </c>
+      <c r="H34">
+        <v>0.59345637149844666</v>
+      </c>
+      <c r="I34">
+        <v>958</v>
+      </c>
+      <c r="J34">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35">
+        <v>0.9</v>
+      </c>
+      <c r="D35" s="5">
+        <v>5.0017486937079694</v>
+      </c>
+      <c r="E35" s="5">
+        <v>7.3985651729296498E-2</v>
+      </c>
+      <c r="F35" s="5">
+        <v>-9.9079417051590693E-2</v>
+      </c>
+      <c r="G35">
+        <v>1.1020561389532419</v>
+      </c>
+      <c r="H35">
+        <v>0.50005899127852116</v>
+      </c>
+      <c r="I35">
+        <v>754</v>
+      </c>
+      <c r="J35">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36">
+        <v>0.9</v>
+      </c>
+      <c r="D36" s="5">
+        <v>2.756452705730716</v>
+      </c>
+      <c r="E36" s="5">
+        <v>4.5983358870907542E-2</v>
+      </c>
+      <c r="F36" s="5">
+        <v>-0.28250362545158608</v>
+      </c>
+      <c r="G36">
+        <v>0.31037546316096543</v>
+      </c>
+      <c r="H36">
+        <v>0.2464362515908195</v>
+      </c>
+      <c r="I36">
+        <v>2160</v>
+      </c>
+      <c r="J36">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37">
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="D37" s="5">
+        <v>2.660620405770405</v>
+      </c>
+      <c r="E37" s="5">
+        <v>4.4343546529255207E-2</v>
+      </c>
+      <c r="F37" s="5">
+        <v>-0.32348322726909851</v>
+      </c>
+      <c r="G37">
+        <v>0.27290132221217428</v>
+      </c>
+      <c r="H37">
+        <v>0.23997716145617429</v>
+      </c>
+      <c r="I37">
+        <v>2511</v>
+      </c>
+      <c r="J37">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38">
+        <v>0.8</v>
+      </c>
+      <c r="D38" s="5">
+        <v>2.4670177218669651</v>
+      </c>
+      <c r="E38" s="5">
+        <v>4.0851064375217787E-2</v>
+      </c>
+      <c r="F38" s="5">
+        <v>-0.31087628330327449</v>
+      </c>
+      <c r="G38">
+        <v>0.2551161941543747</v>
+      </c>
+      <c r="H38">
+        <v>0.21192333097877741</v>
+      </c>
+      <c r="I38">
+        <v>2342</v>
+      </c>
+      <c r="J38">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39">
+        <v>0.6</v>
+      </c>
+      <c r="D39" s="5">
+        <v>2.230995895006</v>
+      </c>
+      <c r="E39" s="5">
+        <v>3.622041501088491E-2</v>
+      </c>
+      <c r="F39" s="5">
+        <v>-0.35832826158481063</v>
+      </c>
+      <c r="G39">
+        <v>0.19755032650523291</v>
+      </c>
+      <c r="H39">
+        <v>0.18003501132421079</v>
+      </c>
+      <c r="I39">
+        <v>2747</v>
+      </c>
+      <c r="J39">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40">
+        <v>0.5</v>
+      </c>
+      <c r="D40" s="5">
+        <v>1.8581415574633591</v>
+      </c>
+      <c r="E40" s="5">
+        <v>2.7852340044160151E-2</v>
+      </c>
+      <c r="F40" s="5">
+        <v>-0.37817862554980769</v>
+      </c>
+      <c r="G40">
+        <v>0.1277952970691294</v>
+      </c>
+      <c r="H40">
+        <v>0.1222948536576836</v>
+      </c>
+      <c r="I40">
+        <v>3015</v>
+      </c>
+      <c r="J40">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="5">
+        <v>1.806541450777194</v>
+      </c>
+      <c r="E41" s="5">
+        <v>2.656965511962861E-2</v>
+      </c>
+      <c r="F41" s="5">
+        <v>-0.66585514620401398</v>
+      </c>
+      <c r="G41">
+        <v>6.3897130191662016E-2</v>
+      </c>
+      <c r="H41">
+        <v>8.3200450875002455E-2</v>
+      </c>
+      <c r="I41" t="s">
+        <v>16</v>
+      </c>
+      <c r="J41">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42">
+        <v>0.2</v>
+      </c>
+      <c r="D42" s="5">
+        <v>1.5421540810388741</v>
+      </c>
+      <c r="E42" s="5">
+        <v>1.9392485824350381E-2</v>
+      </c>
+      <c r="F42" s="5">
+        <v>-0.53260637211956907</v>
+      </c>
+      <c r="G42">
+        <v>6.1267541321923018E-2</v>
+      </c>
+      <c r="H42">
+        <v>6.0174153486635691E-2</v>
+      </c>
+      <c r="I42">
+        <v>3419</v>
+      </c>
+      <c r="J42">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43">
+        <v>0.4</v>
+      </c>
+      <c r="D43" s="5">
+        <v>1.265657123266305</v>
+      </c>
+      <c r="E43" s="5">
+        <v>1.05006772741989E-2</v>
+      </c>
+      <c r="F43" s="5">
+        <v>-0.50112478244064307</v>
+      </c>
+      <c r="G43">
+        <v>4.4131822333190844E-3</v>
+      </c>
+      <c r="H43">
+        <v>4.5054951247551992E-3</v>
+      </c>
+      <c r="I43">
+        <v>3312</v>
+      </c>
+      <c r="J43">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44">
+        <v>0.9</v>
+      </c>
+      <c r="D44" s="5">
+        <v>0.62309783034908539</v>
+      </c>
+      <c r="E44" s="5">
+        <v>-2.0756279343396519E-2</v>
+      </c>
+      <c r="F44" s="5">
+        <v>-0.75379161355641588</v>
+      </c>
+      <c r="G44">
+        <v>-0.21155784257866281</v>
+      </c>
+      <c r="H44">
+        <v>-0.1948685856912071</v>
+      </c>
+      <c r="I44">
+        <v>2882</v>
+      </c>
+      <c r="J44">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45">
+        <v>0.3</v>
+      </c>
+      <c r="D45" s="5">
+        <v>0.47142966756492488</v>
+      </c>
+      <c r="E45" s="5">
+        <v>-3.2792671011872658E-2</v>
+      </c>
+      <c r="F45" s="5">
+        <v>-0.7558993049940842</v>
+      </c>
+      <c r="G45">
+        <v>-0.27038445626377272</v>
+      </c>
+      <c r="H45">
+        <v>-0.29201778518017268</v>
+      </c>
+      <c r="I45">
+        <v>3686</v>
+      </c>
+      <c r="J45">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46">
+        <v>0.8</v>
+      </c>
+      <c r="D46" s="5">
+        <v>0.44013634155167891</v>
+      </c>
+      <c r="E46" s="5">
+        <v>-3.5733773963104398E-2</v>
+      </c>
+      <c r="F46" s="5">
+        <v>-0.79569615711345354</v>
+      </c>
+      <c r="G46">
+        <v>-0.30823030500440829</v>
+      </c>
+      <c r="H46">
+        <v>-0.29554587392109688</v>
+      </c>
+      <c r="I46">
+        <v>3061</v>
+      </c>
+      <c r="J46">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47">
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="D47" s="5">
+        <v>0.3513760736717359</v>
+      </c>
+      <c r="E47" s="5">
+        <v>-4.5315397112016258E-2</v>
+      </c>
+      <c r="F47" s="5">
+        <v>-0.83921590551726355</v>
+      </c>
+      <c r="G47">
+        <v>-0.36457632709844351</v>
+      </c>
+      <c r="H47">
+        <v>-0.36363156815173953</v>
+      </c>
+      <c r="I47">
+        <v>3235</v>
+      </c>
+      <c r="J47">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48">
+        <v>0.6</v>
+      </c>
+      <c r="D48" s="5">
+        <v>0.27198801402427297</v>
+      </c>
+      <c r="E48" s="5">
+        <v>-5.609473356287209E-2</v>
+      </c>
+      <c r="F48" s="5">
+        <v>-0.88471994654893937</v>
+      </c>
+      <c r="G48">
+        <v>-0.42264471379599972</v>
+      </c>
+      <c r="H48">
+        <v>-0.43224801204829311</v>
+      </c>
+      <c r="I48">
+        <v>3421</v>
+      </c>
+      <c r="J48">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49">
+        <v>0.5</v>
+      </c>
+      <c r="D49" s="5">
+        <v>0.2045444223441597</v>
+      </c>
+      <c r="E49" s="5">
+        <v>-6.7946374659157316E-2</v>
+      </c>
+      <c r="F49" s="5">
+        <v>-0.92114905135774083</v>
+      </c>
+      <c r="G49">
+        <v>-0.48667102575955129</v>
+      </c>
+      <c r="H49">
+        <v>-0.52212239810551098</v>
+      </c>
+      <c r="I49">
+        <v>3633</v>
+      </c>
+      <c r="J49">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50">
+        <v>0.4</v>
+      </c>
+      <c r="D50" s="5">
+        <v>0.107604661847504</v>
+      </c>
+      <c r="E50" s="5">
+        <v>-9.4116812499330349E-2</v>
+      </c>
+      <c r="F50" s="5">
+        <v>-0.96034881042902598</v>
+      </c>
+      <c r="G50">
+        <v>-0.63238510556813843</v>
+      </c>
+      <c r="H50">
+        <v>-0.70642662193164185</v>
+      </c>
+      <c r="I50">
+        <v>3887</v>
+      </c>
+      <c r="J50">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51">
+        <v>0.1</v>
+      </c>
+      <c r="D51" s="5">
+        <v>5.8806566188079501E-2</v>
+      </c>
+      <c r="E51" s="5">
+        <v>-0.118063393189225</v>
+      </c>
+      <c r="F51" s="5">
+        <v>-0.96423104416697114</v>
+      </c>
+      <c r="G51">
+        <v>-0.74825121106950943</v>
+      </c>
+      <c r="H51">
+        <v>-0.86188507124903169</v>
+      </c>
+      <c r="I51">
+        <v>4249</v>
+      </c>
+      <c r="J51">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52">
+        <v>0.2</v>
+      </c>
+      <c r="D52" s="5">
+        <v>6.1808392644794742E-2</v>
+      </c>
+      <c r="E52" s="5">
+        <v>-0.1161144086350602</v>
+      </c>
+      <c r="F52" s="5">
+        <v>-0.94936912865960255</v>
+      </c>
+      <c r="G52">
+        <v>-0.75603914096532043</v>
+      </c>
+      <c r="H52">
+        <v>-0.86813676980062804</v>
+      </c>
+      <c r="I52">
+        <v>4161</v>
+      </c>
+      <c r="J52">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53">
+        <v>0.3</v>
+      </c>
+      <c r="D53" s="5">
+        <v>4.6149013287523168E-2</v>
+      </c>
+      <c r="E53" s="5">
+        <v>-0.12749067312912901</v>
+      </c>
+      <c r="F53" s="5">
+        <v>-0.97824934547381892</v>
+      </c>
+      <c r="G53">
+        <v>-0.80887766341804002</v>
+      </c>
+      <c r="H53">
+        <v>-0.93070015696612018</v>
+      </c>
+      <c r="I53">
+        <v>4153</v>
+      </c>
+      <c r="J53">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54">
+        <v>0.2</v>
+      </c>
+      <c r="D54" s="5">
+        <v>1.4526254980643831E-2</v>
+      </c>
+      <c r="E54" s="5">
+        <v>-0.17108226919935809</v>
+      </c>
+      <c r="F54" s="5">
+        <v>-0.991933329546279</v>
+      </c>
+      <c r="G54">
+        <v>-1.031695709403657</v>
+      </c>
+      <c r="H54">
+        <v>-1.2188774466606469</v>
+      </c>
+      <c r="I54">
+        <v>4468</v>
+      </c>
+      <c r="J54">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55">
+        <v>0.1</v>
+      </c>
+      <c r="D55" s="5">
+        <v>7.1270484212235643E-3</v>
+      </c>
+      <c r="E55" s="5">
+        <v>-0.19684417965072529</v>
+      </c>
+      <c r="F55" s="5">
+        <v>-0.99416878093925221</v>
+      </c>
+      <c r="G55">
+        <v>-1.190723824150248</v>
+      </c>
+      <c r="H55">
+        <v>-1.4853163937064029</v>
+      </c>
+      <c r="I55">
+        <v>4674</v>
+      </c>
+      <c r="J55">
+        <v>22.553424657534251</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56">
+        <v>0.1</v>
+      </c>
+      <c r="D56" s="5">
+        <v>2.6015078934843059E-3</v>
+      </c>
+      <c r="E56" s="5">
+        <v>-0.2319433683982253</v>
+      </c>
+      <c r="F56" s="5">
+        <v>-0.99796858354326023</v>
+      </c>
+      <c r="G56">
+        <v>-1.360196441892549</v>
+      </c>
+      <c r="H56">
+        <v>-1.7110563642572489</v>
+      </c>
+      <c r="I56">
+        <v>4858</v>
+      </c>
+      <c r="J56">
+        <v>22.553424657534251</v>
       </c>
     </row>
   </sheetData>
@@ -18693,7 +20539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>